<commit_message>
Additional picture dump for report and presentation
</commit_message>
<xml_diff>
--- a/results/processed/MannerOfDeath_given_IsFullMoon.xlsx
+++ b/results/processed/MannerOfDeath_given_IsFullMoon.xlsx
@@ -46,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -88,7 +88,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,6 +122,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cause of Death given Full Moon</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -209,7 +234,7 @@
                   <c:v>1.65269783948554E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1015044194658093E-4</c:v>
+                  <c:v>7.10150441946581E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.1691761846883201E-4</c:v>
@@ -274,7 +299,7 @@
                   <c:v>1.6292748657647099E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3319045445225665E-4</c:v>
+                  <c:v>5.83190454452257E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0691761846883201E-4</c:v>
@@ -1368,7 +1393,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1401,10 +1426,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>8.1015044194658093E-4</v>
+        <v>7.10150441946581E-4</v>
       </c>
       <c r="C3" s="1">
-        <v>5.3319045445225665E-4</v>
+        <v>5.83190454452257E-4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>